<commit_message>
Piushing airbnbFINAL_JS.csv to branch Jason_Add_Clean_To_Raph
</commit_message>
<xml_diff>
--- a/2018/Suburbs to clean.xlsx
+++ b/2018/Suburbs to clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/J/Documents/Project1/Project1/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49A6EDE-6413-B045-919C-898B552E5A2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448BC3A8-791B-BE48-8889-816EE9DA80B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="500" windowWidth="26280" windowHeight="15940" xr2:uid="{6A67B8A3-2862-8747-9653-65CB8C1F79B1}"/>
   </bookViews>
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>